<commit_message>
Clean up index.html indentation and refactor bubble chart functions
</commit_message>
<xml_diff>
--- a/data/Calls by Neighborhood per capita.xlsx
+++ b/data/Calls by Neighborhood per capita.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Documents/Boston-311-Services/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Documents/Boston-311-Services/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -221,29 +221,29 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,8 +531,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="17" customWidth="1"/>
     <col min="5" max="5" width="28.6640625" style="11" customWidth="1"/>
     <col min="6" max="6" width="28.5" style="9" customWidth="1"/>
     <col min="9" max="10" width="32.6640625" customWidth="1"/>
@@ -546,10 +546,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E1" s="10" t="s">
@@ -585,15 +585,15 @@
       <c r="B2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="17">
-        <f>G2/F2</f>
+      <c r="C2" s="15">
+        <f t="shared" ref="C2:C19" si="0">G2/F2</f>
         <v>7.5782950929492547E-3</v>
       </c>
-      <c r="D2" s="17">
-        <f>H2/F2</f>
+      <c r="D2" s="15">
+        <f t="shared" ref="D2:D19" si="1">H2/F2</f>
         <v>1.1430246189917937E-2</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="12">
         <f>I2/F2</f>
         <v>3.1401775247027297E-3</v>
       </c>
@@ -617,7 +617,7 @@
         <v>54.2</v>
       </c>
       <c r="M2" s="5">
-        <f>K2/L2*100</f>
+        <f t="shared" ref="M2:M19" si="2">K2/L2*100</f>
         <v>49066.420664206642</v>
       </c>
     </row>
@@ -628,16 +628,16 @@
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="17">
-        <f>G3/F3</f>
+      <c r="C3" s="15">
+        <f t="shared" si="0"/>
         <v>0.24512883061442292</v>
       </c>
-      <c r="D3" s="17">
-        <f>H3/F3</f>
+      <c r="D3" s="15">
+        <f t="shared" si="1"/>
         <v>0.3008690349138588</v>
       </c>
-      <c r="E3" s="14">
-        <f t="shared" ref="E3:E19" si="0">I3/F3</f>
+      <c r="E3" s="12">
+        <f t="shared" ref="E3:E19" si="3">I3/F3</f>
         <v>2.7534685165421558E-2</v>
       </c>
       <c r="F3" s="8">
@@ -660,7 +660,7 @@
         <v>55.9</v>
       </c>
       <c r="M3" s="5">
-        <f>K3/L3*100</f>
+        <f t="shared" si="2"/>
         <v>32862.25402504472</v>
       </c>
     </row>
@@ -671,16 +671,16 @@
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="17">
-        <f>G4/F4</f>
+      <c r="C4" s="15">
+        <f t="shared" si="0"/>
         <v>7.5473455448618443E-2</v>
       </c>
-      <c r="D4" s="17">
-        <f>H4/F4</f>
+      <c r="D4" s="15">
+        <f t="shared" si="1"/>
         <v>0.13505122632722757</v>
       </c>
-      <c r="E4" s="14">
-        <f t="shared" si="0"/>
+      <c r="E4" s="12">
+        <f t="shared" si="3"/>
         <v>2.8283141881403292E-2</v>
       </c>
       <c r="F4" s="8">
@@ -703,7 +703,7 @@
         <v>52.4</v>
       </c>
       <c r="M4" s="5">
-        <f>K4/L4*100</f>
+        <f t="shared" si="2"/>
         <v>32255.725190839694</v>
       </c>
     </row>
@@ -714,16 +714,16 @@
       <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="17">
-        <f>G5/F5</f>
+      <c r="C5" s="15">
+        <f t="shared" si="0"/>
         <v>0.18193058873120696</v>
       </c>
-      <c r="D5" s="17">
-        <f>H5/F5</f>
+      <c r="D5" s="15">
+        <f t="shared" si="1"/>
         <v>0.19907264296754251</v>
       </c>
-      <c r="E5" s="14">
-        <f t="shared" si="0"/>
+      <c r="E5" s="12">
+        <f t="shared" si="3"/>
         <v>3.7628214135169313E-2</v>
       </c>
       <c r="F5" s="8">
@@ -746,7 +746,7 @@
         <v>52.1</v>
       </c>
       <c r="M5" s="5">
-        <f>K5/L5*100</f>
+        <f t="shared" si="2"/>
         <v>36095.969289827255</v>
       </c>
     </row>
@@ -757,16 +757,16 @@
       <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17">
-        <f>G6/F6</f>
+      <c r="C6" s="15">
+        <f t="shared" si="0"/>
         <v>0.13752219071564556</v>
       </c>
-      <c r="D6" s="17">
-        <f>H6/F6</f>
+      <c r="D6" s="15">
+        <f t="shared" si="1"/>
         <v>0.14336206411811486</v>
       </c>
-      <c r="E6" s="14">
-        <f t="shared" si="0"/>
+      <c r="E6" s="12">
+        <f t="shared" si="3"/>
         <v>4.389946099655391E-2</v>
       </c>
       <c r="F6" s="8">
@@ -789,7 +789,7 @@
         <v>51.7</v>
       </c>
       <c r="M6" s="5">
-        <f>K6/L6*100</f>
+        <f t="shared" si="2"/>
         <v>124947.77562862668</v>
       </c>
     </row>
@@ -800,16 +800,16 @@
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="17">
-        <f>G7/F7</f>
+      <c r="C7" s="15">
+        <f t="shared" si="0"/>
         <v>0.16941919135788749</v>
       </c>
-      <c r="D7" s="17">
-        <f>H7/F7</f>
+      <c r="D7" s="15">
+        <f t="shared" si="1"/>
         <v>0.18595656716086154</v>
       </c>
-      <c r="E7" s="14">
-        <f t="shared" si="0"/>
+      <c r="E7" s="12">
+        <f t="shared" si="3"/>
         <v>5.1212518615661604E-2</v>
       </c>
       <c r="F7" s="8">
@@ -832,7 +832,7 @@
         <v>46.1</v>
       </c>
       <c r="M7" s="5">
-        <f>K7/L7*100</f>
+        <f t="shared" si="2"/>
         <v>46251.626898047718</v>
       </c>
     </row>
@@ -843,16 +843,16 @@
       <c r="B8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="17">
-        <f>G8/F8</f>
+      <c r="C8" s="15">
+        <f t="shared" si="0"/>
         <v>0.21707862030442676</v>
       </c>
-      <c r="D8" s="17">
-        <f>H8/F8</f>
+      <c r="D8" s="15">
+        <f t="shared" si="1"/>
         <v>0.20618628683144813</v>
       </c>
-      <c r="E8" s="14">
-        <f t="shared" si="0"/>
+      <c r="E8" s="12">
+        <f t="shared" si="3"/>
         <v>5.1878229297584136E-2</v>
       </c>
       <c r="F8" s="8">
@@ -875,7 +875,7 @@
         <v>54.3</v>
       </c>
       <c r="M8" s="5">
-        <f>K8/L8*100</f>
+        <f t="shared" si="2"/>
         <v>29077.348066298346</v>
       </c>
     </row>
@@ -886,16 +886,16 @@
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="17">
-        <f>G9/F9</f>
+      <c r="C9" s="15">
+        <f t="shared" si="0"/>
         <v>0.12526946107784431</v>
       </c>
-      <c r="D9" s="17">
-        <f>H9/F9</f>
+      <c r="D9" s="15">
+        <f t="shared" si="1"/>
         <v>0.15467065868263474</v>
       </c>
-      <c r="E9" s="14">
-        <f t="shared" si="0"/>
+      <c r="E9" s="12">
+        <f t="shared" si="3"/>
         <v>5.4610778443113774E-2</v>
       </c>
       <c r="F9" s="8">
@@ -918,7 +918,7 @@
         <v>48.7</v>
       </c>
       <c r="M9" s="5">
-        <f>K9/L9*100</f>
+        <f t="shared" si="2"/>
         <v>16967.145790554416</v>
       </c>
     </row>
@@ -929,16 +929,16 @@
       <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="17">
-        <f>G10/F10</f>
+      <c r="C10" s="15">
+        <f t="shared" si="0"/>
         <v>0.27505356848524809</v>
       </c>
-      <c r="D10" s="17">
-        <f>H10/F10</f>
+      <c r="D10" s="15">
+        <f t="shared" si="1"/>
         <v>0.29479149497280371</v>
       </c>
-      <c r="E10" s="14">
-        <f t="shared" si="0"/>
+      <c r="E10" s="12">
+        <f t="shared" si="3"/>
         <v>5.6576561727377614E-2</v>
       </c>
       <c r="F10" s="8">
@@ -961,7 +961,7 @@
         <v>51.6</v>
       </c>
       <c r="M10" s="5">
-        <f>K10/L10*100</f>
+        <f t="shared" si="2"/>
         <v>25788.759689922477</v>
       </c>
     </row>
@@ -972,16 +972,16 @@
       <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="17">
-        <f>G11/F11</f>
+      <c r="C11" s="15">
+        <f t="shared" si="0"/>
         <v>0.19044190940303465</v>
       </c>
-      <c r="D11" s="17">
-        <f>H11/F11</f>
+      <c r="D11" s="15">
+        <f t="shared" si="1"/>
         <v>0.24138885812382324</v>
       </c>
-      <c r="E11" s="14">
-        <f t="shared" si="0"/>
+      <c r="E11" s="12">
+        <f t="shared" si="3"/>
         <v>6.0970207110421976E-2</v>
       </c>
       <c r="F11" s="8">
@@ -1004,7 +1004,7 @@
         <v>54.1</v>
       </c>
       <c r="M11" s="5">
-        <f>K11/L11*100</f>
+        <f t="shared" si="2"/>
         <v>18301.293900184843</v>
       </c>
     </row>
@@ -1015,16 +1015,16 @@
       <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="17">
-        <f>G12/F12</f>
+      <c r="C12" s="15">
+        <f t="shared" si="0"/>
         <v>0.20101936799184505</v>
       </c>
-      <c r="D12" s="17">
-        <f>H12/F12</f>
+      <c r="D12" s="15">
+        <f t="shared" si="1"/>
         <v>0.22731906218144751</v>
       </c>
-      <c r="E12" s="14">
-        <f t="shared" si="0"/>
+      <c r="E12" s="12">
+        <f t="shared" si="3"/>
         <v>6.4143730886850159E-2</v>
       </c>
       <c r="F12" s="8">
@@ -1047,7 +1047,7 @@
         <v>55</v>
       </c>
       <c r="M12" s="5">
-        <f>K12/L12*100</f>
+        <f t="shared" si="2"/>
         <v>39181.818181818184</v>
       </c>
     </row>
@@ -1058,16 +1058,16 @@
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="17">
-        <f>G13/F13</f>
+      <c r="C13" s="15">
+        <f t="shared" si="0"/>
         <v>0.19614844298759074</v>
       </c>
-      <c r="D13" s="17">
-        <f>H13/F13</f>
+      <c r="D13" s="15">
+        <f t="shared" si="1"/>
         <v>0.23841020838211191</v>
       </c>
-      <c r="E13" s="14">
-        <f t="shared" si="0"/>
+      <c r="E13" s="12">
+        <f t="shared" si="3"/>
         <v>6.990946694763131E-2</v>
       </c>
       <c r="F13" s="8">
@@ -1090,7 +1090,7 @@
         <v>52.2</v>
       </c>
       <c r="M13" s="5">
-        <f>K13/L13*100</f>
+        <f t="shared" si="2"/>
         <v>51731.80076628353</v>
       </c>
     </row>
@@ -1101,16 +1101,16 @@
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="17">
-        <f>G14/F14</f>
+      <c r="C14" s="15">
+        <f t="shared" si="0"/>
         <v>0.19497949223820155</v>
       </c>
-      <c r="D14" s="17">
-        <f>H14/F14</f>
+      <c r="D14" s="15">
+        <f t="shared" si="1"/>
         <v>0.19726390114739628</v>
       </c>
-      <c r="E14" s="14">
-        <f t="shared" si="0"/>
+      <c r="E14" s="12">
+        <f t="shared" si="3"/>
         <v>0.10022844089091948</v>
       </c>
       <c r="F14" s="8">
@@ -1133,7 +1133,7 @@
         <v>51.2</v>
       </c>
       <c r="M14" s="5">
-        <f>K14/L14*100</f>
+        <f t="shared" si="2"/>
         <v>35458.984375</v>
       </c>
     </row>
@@ -1144,16 +1144,16 @@
       <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="17">
-        <f>G15/F15</f>
+      <c r="C15" s="15">
+        <f t="shared" si="0"/>
         <v>0.13290718648144045</v>
       </c>
-      <c r="D15" s="17">
-        <f>H15/F15</f>
+      <c r="D15" s="15">
+        <f t="shared" si="1"/>
         <v>0.15072307838359544</v>
       </c>
-      <c r="E15" s="14">
-        <f t="shared" si="0"/>
+      <c r="E15" s="12">
+        <f t="shared" si="3"/>
         <v>0.1079079775956457</v>
       </c>
       <c r="F15" s="8">
@@ -1176,7 +1176,7 @@
         <v>49.8</v>
       </c>
       <c r="M15" s="5">
-        <f>K15/L15*100</f>
+        <f t="shared" si="2"/>
         <v>31907.630522088359</v>
       </c>
     </row>
@@ -1187,16 +1187,16 @@
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="17">
-        <f>G16/F16</f>
+      <c r="C16" s="15">
+        <f t="shared" si="0"/>
         <v>0.48636202621324831</v>
       </c>
-      <c r="D16" s="17">
-        <f>H16/F16</f>
+      <c r="D16" s="15">
+        <f t="shared" si="1"/>
         <v>0.53403167855877742</v>
       </c>
-      <c r="E16" s="14">
-        <f t="shared" si="0"/>
+      <c r="E16" s="12">
+        <f t="shared" si="3"/>
         <v>0.16279540509083548</v>
       </c>
       <c r="F16" s="8">
@@ -1219,7 +1219,7 @@
         <v>51.4</v>
       </c>
       <c r="M16" s="5">
-        <f>K16/L16*100</f>
+        <f t="shared" si="2"/>
         <v>19389.10505836576</v>
       </c>
     </row>
@@ -1230,16 +1230,16 @@
       <c r="B17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="17">
-        <f>G17/F17</f>
+      <c r="C17" s="15">
+        <f t="shared" si="0"/>
         <v>0.26164874551971329</v>
       </c>
-      <c r="D17" s="17">
-        <f>H17/F17</f>
+      <c r="D17" s="15">
+        <f t="shared" si="1"/>
         <v>0.27678215850258864</v>
       </c>
-      <c r="E17" s="14">
-        <f t="shared" si="0"/>
+      <c r="E17" s="12">
+        <f t="shared" si="3"/>
         <v>0.19525516299709847</v>
       </c>
       <c r="F17" s="8">
@@ -1262,7 +1262,7 @@
         <v>52.8</v>
       </c>
       <c r="M17" s="5">
-        <f>K17/L17*100</f>
+        <f t="shared" si="2"/>
         <v>18164.772727272728</v>
       </c>
     </row>
@@ -1273,16 +1273,16 @@
       <c r="B18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="17">
-        <f>G18/F18</f>
+      <c r="C18" s="15">
+        <f t="shared" si="0"/>
         <v>0.3230787434183281</v>
       </c>
-      <c r="D18" s="17">
-        <f>H18/F18</f>
+      <c r="D18" s="15">
+        <f t="shared" si="1"/>
         <v>0.30592202567591553</v>
       </c>
-      <c r="E18" s="14">
-        <f t="shared" si="0"/>
+      <c r="E18" s="12">
+        <f t="shared" si="3"/>
         <v>0.21682541560669705</v>
       </c>
       <c r="F18" s="8">
@@ -1305,7 +1305,7 @@
         <v>49.3</v>
       </c>
       <c r="M18" s="5">
-        <f>K18/L18*100</f>
+        <f t="shared" si="2"/>
         <v>17389.452332657202</v>
       </c>
     </row>
@@ -1316,16 +1316,16 @@
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="17">
-        <f>G19/F19</f>
+      <c r="C19" s="15">
+        <f t="shared" si="0"/>
         <v>0.22622246104245031</v>
       </c>
-      <c r="D19" s="17">
-        <f>H19/F19</f>
+      <c r="D19" s="15">
+        <f t="shared" si="1"/>
         <v>0.37710908113917246</v>
       </c>
-      <c r="E19" s="14">
-        <f t="shared" si="0"/>
+      <c r="E19" s="12">
+        <f t="shared" si="3"/>
         <v>0.29564750134336376</v>
       </c>
       <c r="F19" s="8">
@@ -1348,50 +1348,50 @@
         <v>53.6</v>
       </c>
       <c r="M19" s="5">
-        <f>K19/L19*100</f>
+        <f t="shared" si="2"/>
         <v>9210.8208955223872</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="18"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="16"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>